<commit_message>
tentativa de por a calculadora
</commit_message>
<xml_diff>
--- a/bi/minha_carteira.xlsx
+++ b/bi/minha_carteira.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff\Desktop\GITHUB\cotacaopython\bi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69117A96-1BE8-4D86-9630-87481DEB7A5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD9FDED-429C-4C60-939D-CFB334F497FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11200" yWindow="4260" windowWidth="14480" windowHeight="15870" xr2:uid="{BA8CCB60-0BDB-486D-9217-0F76718954BB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{BA8CCB60-0BDB-486D-9217-0F76718954BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -118,9 +118,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,7 +436,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4F918FA-71C0-496A-8C75-589E0000FF18}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
@@ -534,6 +535,9 @@
       <c r="D6" s="1">
         <v>31</v>
       </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B8" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C6">

</xml_diff>